<commit_message>
jan6 stable, with weird low kappa results
</commit_message>
<xml_diff>
--- a/formatted_output/twostagedc_ef_nov25.xlsx
+++ b/formatted_output/twostagedc_ef_nov25.xlsx
@@ -478,22 +478,22 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>206.9680344307237</v>
+        <v>207.6771426899587</v>
       </c>
       <c r="D2" t="n">
-        <v>664.0722795128331</v>
+        <v>670.7147553898792</v>
       </c>
       <c r="E2" t="n">
-        <v>577.4401890364425</v>
+        <v>577.812872910898</v>
       </c>
       <c r="F2" t="n">
-        <v>58.28964996337891</v>
+        <v>58.27642440795898</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2604723125696182</v>
+        <v>0.2681797484556834</v>
       </c>
       <c r="H2" t="n">
-        <v>-12.34535964543473</v>
+        <v>-12.27697058012694</v>
       </c>
     </row>
     <row r="3">
@@ -504,22 +504,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>233.7534601731711</v>
+        <v>237.4366042710649</v>
       </c>
       <c r="D3" t="n">
-        <v>751.863808344764</v>
+        <v>777.0465877804547</v>
       </c>
       <c r="E3" t="n">
-        <v>627.62355161559</v>
+        <v>632.593492344443</v>
       </c>
       <c r="F3" t="n">
-        <v>56.54822158813477</v>
+        <v>56.47904968261719</v>
       </c>
       <c r="G3" t="n">
-        <v>0.297820786635081</v>
+        <v>0.3011502499381701</v>
       </c>
       <c r="H3" t="n">
-        <v>-8.959941902011616</v>
+        <v>-8.791913332040506</v>
       </c>
     </row>
     <row r="4">
@@ -530,22 +530,22 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>262.0333243230311</v>
+        <v>260.9055146073916</v>
       </c>
       <c r="D4" t="n">
-        <v>744.6882752653125</v>
+        <v>769.0957211901207</v>
       </c>
       <c r="E4" t="n">
-        <v>627.6835416627921</v>
+        <v>635.6250120368361</v>
       </c>
       <c r="F4" t="n">
-        <v>55.70576095581055</v>
+        <v>55.71476745605469</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2962281808257103</v>
+        <v>0.2891035795211792</v>
       </c>
       <c r="H4" t="n">
-        <v>-7.057813613124524</v>
+        <v>-7.110600690419609</v>
       </c>
     </row>
     <row r="5">
@@ -556,22 +556,22 @@
         <v>15</v>
       </c>
       <c r="C5" t="n">
-        <v>272.2499541229236</v>
+        <v>272.3699359732539</v>
       </c>
       <c r="D5" t="n">
-        <v>748.9761735849014</v>
+        <v>808.2246944543577</v>
       </c>
       <c r="E5" t="n">
-        <v>633.3642749612982</v>
+        <v>649.313825610144</v>
       </c>
       <c r="F5" t="n">
-        <v>55.23115158081055</v>
+        <v>55.15425109863281</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3030264263351758</v>
+        <v>0.3258351335922877</v>
       </c>
       <c r="H5" t="n">
-        <v>-6.440120604155975</v>
+        <v>-6.424721521794428</v>
       </c>
     </row>
     <row r="6">
@@ -582,22 +582,22 @@
         <v>20</v>
       </c>
       <c r="C6" t="n">
-        <v>277.7005599003273</v>
+        <v>277.627585341904</v>
       </c>
       <c r="D6" t="n">
-        <v>777.730477571913</v>
+        <v>811.7768842965512</v>
       </c>
       <c r="E6" t="n">
-        <v>648.4428384731676</v>
+        <v>656.3094173192217</v>
       </c>
       <c r="F6" t="n">
-        <v>54.86610412597656</v>
+        <v>54.79643249511719</v>
       </c>
       <c r="G6" t="n">
-        <v>0.312116044263045</v>
+        <v>0.3240887582302093</v>
       </c>
       <c r="H6" t="n">
-        <v>-6.126849586540684</v>
+        <v>-6.13164976385664</v>
       </c>
     </row>
     <row r="7">
@@ -608,22 +608,22 @@
         <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>283.7010842867932</v>
+        <v>385.4156814203054</v>
       </c>
       <c r="D7" t="n">
-        <v>808.8915401875319</v>
+        <v>760.6041108193398</v>
       </c>
       <c r="E7" t="n">
-        <v>658.7729391424673</v>
+        <v>666.8098509206569</v>
       </c>
       <c r="F7" t="n">
-        <v>54.31085586547852</v>
+        <v>52.40727615356445</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3112760921319326</v>
+        <v>0.2526679933071136</v>
       </c>
       <c r="H7" t="n">
-        <v>-5.815186928124586</v>
+        <v>-1.328868571424224</v>
       </c>
     </row>
     <row r="8">
@@ -634,22 +634,22 @@
         <v>50</v>
       </c>
       <c r="C8" t="n">
-        <v>381.4887236061165</v>
+        <v>383.5409078367964</v>
       </c>
       <c r="D8" t="n">
-        <v>765.0166040551323</v>
+        <v>758.7175875679043</v>
       </c>
       <c r="E8" t="n">
-        <v>658.1777745434434</v>
+        <v>664.302173300609</v>
       </c>
       <c r="F8" t="n">
-        <v>52.76097106933594</v>
+        <v>52.44415664672852</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2554553906122843</v>
+        <v>0.2526491582393646</v>
       </c>
       <c r="H8" t="n">
-        <v>-1.348237652924793</v>
+        <v>-1.308050690732231</v>
       </c>
     </row>
     <row r="9">
@@ -660,22 +660,22 @@
         <v>200</v>
       </c>
       <c r="C9" t="n">
-        <v>405.0221835797222</v>
+        <v>406.3610972076485</v>
       </c>
       <c r="D9" t="n">
-        <v>782.630094876617</v>
+        <v>778.1885662067625</v>
       </c>
       <c r="E9" t="n">
-        <v>696.3254015356183</v>
+        <v>696.3223353070689</v>
       </c>
       <c r="F9" t="n">
-        <v>50.37053298950195</v>
+        <v>50.11466979980469</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2282893354694049</v>
+        <v>0.2197113633155823</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.9602902872635558</v>
+        <v>-0.9550680434734532</v>
       </c>
     </row>
     <row r="10">
@@ -686,22 +686,22 @@
         <v>2000</v>
       </c>
       <c r="C10" t="n">
-        <v>423.7081931221801</v>
+        <v>424.2297795461056</v>
       </c>
       <c r="D10" t="n">
-        <v>839.5675247764652</v>
+        <v>840.2539961103175</v>
       </c>
       <c r="E10" t="n">
-        <v>764.4444088361513</v>
+        <v>766.1450757336813</v>
       </c>
       <c r="F10" t="n">
-        <v>46.89864730834961</v>
+        <v>46.74080276489258</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2096879775325457</v>
+        <v>0.2077515870332718</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.8595081806537471</v>
+        <v>-0.8646137478218536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>